<commit_message>
Added a requirements comment
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\facultate\anul_3_sem_2\vvss\lab\DeltaPlan\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17FA11D-72D6-4A7B-A4F6-0DF8EE0D39CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BEA4125-BAF3-48C4-8F98-BC2B1E706FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="38">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -141,6 +141,40 @@
   </si>
   <si>
     <t>Halbeș Cătălin</t>
+  </si>
+  <si>
+    <t>R02</t>
+  </si>
+  <si>
+    <t>01. (possibly F02)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">App misses a functionality to view </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>all</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tasks</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -362,6 +396,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -404,7 +439,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -749,7 +783,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -769,19 +803,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -794,7 +828,7 @@
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="35" t="s">
+      <c r="I3" s="21" t="s">
         <v>33</v>
       </c>
       <c r="J3" s="17">
@@ -805,14 +839,14 @@
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="24"/>
+      <c r="E4" s="25"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="35" t="s">
+      <c r="I4" s="21" t="s">
         <v>34</v>
       </c>
       <c r="J4" s="3">
@@ -823,10 +857,10 @@
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="26"/>
+      <c r="E5" s="27"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -838,15 +872,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
@@ -866,9 +900,15 @@
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="2"/>
+      <c r="C10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
@@ -1053,19 +1093,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1078,7 +1118,7 @@
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="35" t="s">
+      <c r="I3" s="21" t="s">
         <v>33</v>
       </c>
       <c r="J3" s="17">
@@ -1089,14 +1129,14 @@
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="27"/>
+      <c r="E4" s="28"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="35" t="s">
+      <c r="I4" s="21" t="s">
         <v>34</v>
       </c>
       <c r="J4" s="3">
@@ -1107,10 +1147,10 @@
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="29"/>
+      <c r="E5" s="30"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -1122,15 +1162,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
@@ -1347,19 +1387,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1372,7 +1412,7 @@
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="35" t="s">
+      <c r="I3" s="21" t="s">
         <v>33</v>
       </c>
       <c r="J3" s="17">
@@ -1383,14 +1423,14 @@
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="30"/>
+      <c r="E4" s="31"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="35" t="s">
+      <c r="I4" s="21" t="s">
         <v>34</v>
       </c>
       <c r="J4" s="3">
@@ -1401,10 +1441,10 @@
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="32"/>
+      <c r="E5" s="33"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -1416,15 +1456,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
@@ -1678,19 +1718,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1703,7 +1743,7 @@
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="35" t="s">
+      <c r="I3" s="21" t="s">
         <v>33</v>
       </c>
       <c r="J3" s="17">
@@ -1714,12 +1754,12 @@
       <c r="C4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="35" t="s">
+      <c r="I4" s="21" t="s">
         <v>34</v>
       </c>
       <c r="J4" s="3">
@@ -1730,8 +1770,8 @@
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -1743,8 +1783,8 @@
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
       <c r="F6" s="20"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -1974,11 +2014,11 @@
       <c r="F30" s="2"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C32" s="33" t="s">
+      <c r="C32" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
       <c r="F32" s="18"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added architecture observations to review report
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\.teme\VVSS\DeltaPlan\Docs\Lab01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\facultate\anul_3_sem_2\vvss\lab\DeltaPlan\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE1651AF-FFE0-4A2B-B7BC-4575AF3614C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B303E430-24A1-4681-A59E-63C4E9487A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2490" yWindow="2160" windowWidth="21600" windowHeight="11385" tabRatio="650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="50">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -202,6 +202,27 @@
   </si>
   <si>
     <t>The requirements do not specify: the file that contains the tasks, which file will be chosen in case a text and a binary file both exist and when the file is loaded</t>
+  </si>
+  <si>
+    <t>A02</t>
+  </si>
+  <si>
+    <t>ClassDiagramTasks</t>
+  </si>
+  <si>
+    <t>A07</t>
+  </si>
+  <si>
+    <t>DateService class name does not seem to reflect the played role</t>
+  </si>
+  <si>
+    <t>DateService has TasksService in composition despite not apparently using it</t>
+  </si>
+  <si>
+    <t>A01</t>
+  </si>
+  <si>
+    <t>The diagram does not clearly illustrate packages or decomposition into subsystems.</t>
   </si>
 </sst>
 </file>
@@ -424,6 +445,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -466,7 +488,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,7 +506,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Temă Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -810,40 +831,40 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="6"/>
-    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.28515625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.85546875" style="6"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.88671875" style="6"/>
     <col min="9" max="9" width="21" style="6" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="6"/>
+    <col min="10" max="10" width="14.44140625" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="24" t="s">
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -852,7 +873,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
@@ -863,14 +884,14 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="25"/>
+      <c r="E4" s="26"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -881,36 +902,36 @@
         <v>233</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="27"/>
+      <c r="E5" s="28"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -924,7 +945,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -938,7 +959,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -946,14 +967,14 @@
       <c r="C11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="36" t="s">
+      <c r="D11" s="22" t="s">
         <v>39</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
@@ -961,14 +982,14 @@
       <c r="C12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="36" t="s">
+      <c r="D12" s="22" t="s">
         <v>39</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -977,7 +998,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -986,7 +1007,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -995,7 +1016,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1004,7 +1025,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1013,7 +1034,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1022,7 +1043,7 @@
       <c r="D18" s="3"/>
       <c r="E18" s="15"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1031,7 +1052,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="15"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1040,7 +1061,7 @@
       <c r="D20" s="3"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1049,7 +1070,7 @@
       <c r="D21" s="3"/>
       <c r="E21" s="15"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1058,7 +1079,7 @@
       <c r="D22" s="3"/>
       <c r="E22" s="15"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1067,7 +1088,7 @@
       <c r="D23" s="3"/>
       <c r="E23" s="15"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1076,7 +1097,7 @@
       <c r="D24" s="3"/>
       <c r="E24" s="15"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1085,12 +1106,14 @@
       <c r="D25" s="3"/>
       <c r="E25" s="15"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C27" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D27" s="12"/>
-      <c r="E27" s="1"/>
+      <c r="E27" s="1">
+        <v>1.5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1113,39 +1136,40 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:J4"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="6"/>
-    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.28515625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.85546875" style="6"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.88671875" style="6"/>
     <col min="9" max="9" width="22" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="6"/>
+    <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="24" t="s">
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1154,7 +1178,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
@@ -1165,14 +1189,14 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="28"/>
+      <c r="E4" s="29"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -1183,36 +1207,36 @@
         <v>233</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="30"/>
+      <c r="E5" s="31"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1226,33 +1250,51 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1261,7 +1303,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1270,7 +1312,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1279,7 +1321,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1288,7 +1330,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1297,7 +1339,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1306,7 +1348,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1315,7 +1357,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1324,7 +1366,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1333,7 +1375,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1342,7 +1384,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1351,7 +1393,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1360,7 +1402,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1369,7 +1411,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1378,12 +1420,14 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C28" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D28" s="12"/>
-      <c r="E28" s="1"/>
+      <c r="E28" s="1">
+        <v>1.5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1406,40 +1450,40 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:J4"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="6"/>
-    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
     <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.85546875" style="6"/>
-    <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="6"/>
+    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.88671875" style="6"/>
+    <col min="9" max="9" width="26.6640625" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="24" t="s">
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1448,7 +1492,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
@@ -1459,14 +1503,14 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="31"/>
+      <c r="E4" s="32"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -1477,36 +1521,36 @@
         <v>233</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="33"/>
+      <c r="E5" s="34"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1520,7 +1564,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1528,7 +1572,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1537,7 +1581,7 @@
       <c r="D11" s="1"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
@@ -1546,7 +1590,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1555,7 +1599,7 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1564,7 +1608,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1573,7 +1617,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1582,7 +1626,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1591,7 +1635,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1600,7 +1644,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1609,7 +1653,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1618,7 +1662,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1627,7 +1671,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1636,7 +1680,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1645,7 +1689,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1654,7 +1698,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1663,7 +1707,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1672,7 +1716,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1681,7 +1725,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1690,7 +1734,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1699,7 +1743,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1708,7 +1752,7 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C32" s="11" t="s">
         <v>8</v>
       </c>
@@ -1740,37 +1784,37 @@
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="6"/>
-    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
     <col min="4" max="4" width="18" style="6" customWidth="1"/>
     <col min="5" max="5" width="24" style="6" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" style="6" customWidth="1"/>
-    <col min="7" max="8" width="8.85546875" style="6"/>
-    <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="6"/>
+    <col min="6" max="6" width="16.6640625" style="6" customWidth="1"/>
+    <col min="7" max="8" width="8.88671875" style="6"/>
+    <col min="9" max="9" width="26.6640625" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="24" t="s">
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1779,7 +1823,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
@@ -1790,12 +1834,12 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -1806,28 +1850,28 @@
         <v>233</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
       <c r="F6" s="20"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1844,7 +1888,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1853,7 +1897,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1863,7 +1907,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
@@ -1873,7 +1917,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1883,7 +1927,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1893,7 +1937,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1903,7 +1947,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1913,7 +1957,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1923,7 +1967,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1933,7 +1977,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1943,7 +1987,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1953,7 +1997,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1963,7 +2007,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1973,7 +2017,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1983,7 +2027,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1993,7 +2037,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2003,7 +2047,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2013,7 +2057,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2023,7 +2067,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2033,7 +2077,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2043,7 +2087,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2053,12 +2097,12 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C32" s="34" t="s">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C32" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
       <c r="F32" s="18"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Used sonarlint, fixed some problems
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\facultate\anul_3_sem_2\vvss\lab\DeltaPlan\Docs\Lab01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\.teme\VVSS\DeltaPlan\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B303E430-24A1-4681-A59E-63C4E9487A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02144C4-8996-4605-803F-A9EBA95EBF00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3390" yWindow="2520" windowWidth="21600" windowHeight="11385" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="67">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -223,6 +223,57 @@
   </si>
   <si>
     <t>The diagram does not clearly illustrate packages or decomposition into subsystems.</t>
+  </si>
+  <si>
+    <t>SonarLint</t>
+  </si>
+  <si>
+    <t>clone should not be overridden</t>
+  </si>
+  <si>
+    <t>clone method was overridden</t>
+  </si>
+  <si>
+    <t>Task.java, 175</t>
+  </si>
+  <si>
+    <t>clone method override implementation was removed</t>
+  </si>
+  <si>
+    <t>TaskIO.java, 18, 19, 20</t>
+  </si>
+  <si>
+    <t>Constant names should comply with a naming convention</t>
+  </si>
+  <si>
+    <t>secondsInDay, secondsInHour, secondsInMin</t>
+  </si>
+  <si>
+    <t>SECONDS_IN_DAY, SECONDS_IN_HOUR, SECONDS_IN_MIN</t>
+  </si>
+  <si>
+    <t>TaskIO.java, 25, 47, 73, 87, 123, 136</t>
+  </si>
+  <si>
+    <t>Try-with-resources should be used</t>
+  </si>
+  <si>
+    <t>finally clause used</t>
+  </si>
+  <si>
+    <t>used try-with-resources + solved possible NullPointerExceptions</t>
+  </si>
+  <si>
+    <t>TaskIO.java, 15</t>
+  </si>
+  <si>
+    <t>Utility classes should not have public constructors</t>
+  </si>
+  <si>
+    <t>no explicit constructor</t>
+  </si>
+  <si>
+    <t>added private constructor</t>
   </si>
 </sst>
 </file>
@@ -506,7 +557,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Temă Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -831,23 +882,23 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="6"/>
-    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.88671875" style="6"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.85546875" style="6"/>
     <col min="9" max="9" width="21" style="6" customWidth="1"/>
-    <col min="10" max="10" width="14.44140625" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="6"/>
+    <col min="10" max="10" width="14.42578125" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -858,7 +909,7 @@
       <c r="I1" s="24"/>
       <c r="J1" s="24"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" s="25" t="s">
         <v>19</v>
       </c>
@@ -873,7 +924,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
@@ -884,7 +935,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
@@ -902,7 +953,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
@@ -916,7 +967,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
@@ -924,14 +975,14 @@
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="23"/>
       <c r="E7" s="23"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -945,7 +996,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -959,7 +1010,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -974,7 +1025,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
@@ -989,7 +1040,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -998,7 +1049,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1007,7 +1058,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1016,7 +1067,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1025,7 +1076,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1034,7 +1085,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1043,7 +1094,7 @@
       <c r="D18" s="3"/>
       <c r="E18" s="15"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1052,7 +1103,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="15"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1061,7 +1112,7 @@
       <c r="D20" s="3"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1070,7 +1121,7 @@
       <c r="D21" s="3"/>
       <c r="E21" s="15"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1079,7 +1130,7 @@
       <c r="D22" s="3"/>
       <c r="E22" s="15"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1088,7 +1139,7 @@
       <c r="D23" s="3"/>
       <c r="E23" s="15"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1097,7 +1148,7 @@
       <c r="D24" s="3"/>
       <c r="E24" s="15"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1106,7 +1157,7 @@
       <c r="D25" s="3"/>
       <c r="E25" s="15"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C27" s="11" t="s">
         <v>8</v>
       </c>
@@ -1136,23 +1187,23 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="6"/>
-    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="17.77734375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.88671875" style="6"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.85546875" style="6"/>
     <col min="9" max="9" width="22" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="6"/>
+    <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -1163,7 +1214,7 @@
       <c r="I1" s="24"/>
       <c r="J1" s="24"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" s="25" t="s">
         <v>18</v>
       </c>
@@ -1178,7 +1229,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
@@ -1189,7 +1240,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
@@ -1207,7 +1258,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
@@ -1221,7 +1272,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
@@ -1229,14 +1280,14 @@
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="23"/>
       <c r="E7" s="23"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1250,7 +1301,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1264,7 +1315,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1279,7 +1330,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
@@ -1294,7 +1345,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1303,7 +1354,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1312,7 +1363,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1321,7 +1372,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1330,7 +1381,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1339,7 +1390,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1348,7 +1399,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1357,7 +1408,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1366,7 +1417,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1375,7 +1426,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1384,7 +1435,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1393,7 +1444,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1402,7 +1453,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1411,7 +1462,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1420,7 +1471,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C28" s="11" t="s">
         <v>8</v>
       </c>
@@ -1450,23 +1501,23 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="6"/>
-    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
     <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.88671875" style="6"/>
-    <col min="9" max="9" width="26.6640625" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="6"/>
+    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.85546875" style="6"/>
+    <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -1477,7 +1528,7 @@
       <c r="I1" s="24"/>
       <c r="J1" s="24"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" s="25" t="s">
         <v>17</v>
       </c>
@@ -1492,7 +1543,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
@@ -1503,7 +1554,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
@@ -1521,7 +1572,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
@@ -1535,7 +1586,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
@@ -1543,14 +1594,14 @@
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="23"/>
       <c r="E7" s="23"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1564,7 +1615,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1572,7 +1623,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1581,7 +1632,7 @@
       <c r="D11" s="1"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
@@ -1590,7 +1641,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1599,7 +1650,7 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1608,7 +1659,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1617,7 +1668,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1626,7 +1677,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1635,7 +1686,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1644,7 +1695,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1653,7 +1704,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1662,7 +1713,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1671,7 +1722,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1680,7 +1731,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1689,7 +1740,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1698,7 +1749,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1707,7 +1758,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1716,7 +1767,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1725,7 +1776,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1734,7 +1785,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1743,7 +1794,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1752,7 +1803,7 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C32" s="11" t="s">
         <v>8</v>
       </c>
@@ -1780,24 +1831,24 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="6"/>
-    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
     <col min="4" max="4" width="18" style="6" customWidth="1"/>
     <col min="5" max="5" width="24" style="6" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" style="6" customWidth="1"/>
-    <col min="7" max="8" width="8.88671875" style="6"/>
-    <col min="9" max="9" width="26.6640625" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="6"/>
+    <col min="6" max="6" width="16.7109375" style="6" customWidth="1"/>
+    <col min="7" max="8" width="8.85546875" style="6"/>
+    <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -1808,7 +1859,7 @@
       <c r="I1" s="24"/>
       <c r="J1" s="24"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" s="25" t="s">
         <v>31</v>
       </c>
@@ -1823,7 +1874,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
@@ -1834,11 +1885,13 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="32"/>
+      <c r="D4" s="32" t="s">
+        <v>50</v>
+      </c>
       <c r="E4" s="32"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
@@ -1850,7 +1903,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
@@ -1862,7 +1915,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>1</v>
@@ -1871,7 +1924,7 @@
       <c r="E6" s="23"/>
       <c r="F6" s="20"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1888,46 +1941,78 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1937,7 +2022,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1947,7 +2032,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1957,7 +2042,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1967,7 +2052,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1977,7 +2062,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1987,7 +2072,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1997,7 +2082,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2007,7 +2092,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2017,7 +2102,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2027,7 +2112,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2037,7 +2122,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2047,7 +2132,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2057,7 +2142,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2067,7 +2152,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2077,7 +2162,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2087,7 +2172,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2097,7 +2182,7 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C32" s="35" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
Performed code review; completed report
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\.teme\VVSS\DeltaPlan\Docs\Lab01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\facultate\anul_3_sem_2\vvss\lab\DeltaPlan\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02144C4-8996-4605-803F-A9EBA95EBF00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC2E14B0-07CF-47E9-B1FB-CDB936CCA5D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3390" yWindow="2520" windowWidth="21600" windowHeight="11385" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="82">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -274,6 +274,51 @@
   </si>
   <si>
     <t>added private constructor</t>
+  </si>
+  <si>
+    <t>21.03.2023</t>
+  </si>
+  <si>
+    <t>C06</t>
+  </si>
+  <si>
+    <t>Controller.java,96</t>
+  </si>
+  <si>
+    <t>NewEditController.java, 149</t>
+  </si>
+  <si>
+    <t>C01</t>
+  </si>
+  <si>
+    <t>code assumes that if an item is selected, edit was pressed - tied to shared logic between new/edit =&gt; don't pass currentTask on pressing "new"</t>
+  </si>
+  <si>
+    <t>selectedItem can be null - errors when trying to edit Task - tied to shared logic between new/edit =&gt; perform null check before casting possible null to Task</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Task.java, 69, 87</t>
+  </si>
+  <si>
+    <t>setTime is unused (overload with signature Date is not even defined in architecture???) =&gt; replace duplicate logic with call to corresponding setTime implementation</t>
+  </si>
+  <si>
+    <t>ArrayTaskList.java, 55</t>
+  </si>
+  <si>
+    <t>improper null check =&gt; replace equals method with == operator</t>
+  </si>
+  <si>
+    <t>21.03.2022</t>
+  </si>
+  <si>
+    <t>17.03.2023</t>
+  </si>
+  <si>
+    <t>13.03.2023</t>
   </si>
 </sst>
 </file>
@@ -557,7 +602,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Temă Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -882,8 +927,8 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -979,7 +1024,9 @@
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="23"/>
+      <c r="D7" s="23" t="s">
+        <v>81</v>
+      </c>
       <c r="E7" s="23"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1188,7 +1235,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="D7" sqref="D7:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1284,7 +1331,9 @@
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="23"/>
+      <c r="D7" s="23" t="s">
+        <v>80</v>
+      </c>
       <c r="E7" s="23"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1598,7 +1647,9 @@
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="23"/>
+      <c r="D7" s="23" t="s">
+        <v>67</v>
+      </c>
       <c r="E7" s="23"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1615,40 +1666,64 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C12" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="C13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
@@ -1808,7 +1883,9 @@
         <v>8</v>
       </c>
       <c r="D32" s="12"/>
-      <c r="E32" s="1"/>
+      <c r="E32" s="1">
+        <v>0.5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1831,8 +1908,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1920,7 +1997,9 @@
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="23"/>
+      <c r="D6" s="23" t="s">
+        <v>79</v>
+      </c>
       <c r="E6" s="23"/>
       <c r="F6" s="20"/>
     </row>
@@ -2188,7 +2267,9 @@
       </c>
       <c r="D32" s="36"/>
       <c r="E32" s="36"/>
-      <c r="F32" s="18"/>
+      <c r="F32" s="18">
+        <v>0.5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Applied some architectural recommendations
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\facultate\anul_3_sem_2\vvss\lab\DeltaPlan\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC2E14B0-07CF-47E9-B1FB-CDB936CCA5D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482B0090-FE0E-4EB9-B9C3-28A3264440EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -213,12 +213,6 @@
     <t>A07</t>
   </si>
   <si>
-    <t>DateService class name does not seem to reflect the played role</t>
-  </si>
-  <si>
-    <t>DateService has TasksService in composition despite not apparently using it</t>
-  </si>
-  <si>
     <t>A01</t>
   </si>
   <si>
@@ -319,6 +313,12 @@
   </si>
   <si>
     <t>13.03.2023</t>
+  </si>
+  <si>
+    <t>DateService/TasksService classes are named 'service' despite apparently playing an utility role</t>
+  </si>
+  <si>
+    <t>TasksService class makes use of ObservableList class from presentation/UI layer (from third-party package JavaFX, even)</t>
   </si>
 </sst>
 </file>
@@ -927,7 +927,7 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
@@ -1025,7 +1025,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E7" s="23"/>
     </row>
@@ -1234,8 +1234,8 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1332,7 +1332,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E7" s="23"/>
     </row>
@@ -1350,7 +1350,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1361,10 +1361,10 @@
         <v>44</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1376,7 +1376,7 @@
         <v>44</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1385,13 +1385,13 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>44</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1648,7 +1648,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E7" s="23"/>
     </row>
@@ -1671,13 +1671,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1686,13 +1686,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1701,13 +1701,13 @@
         <v>3</v>
       </c>
       <c r="C12" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1716,13 +1716,13 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1967,7 +1967,7 @@
         <v>25</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E4" s="32"/>
       <c r="H4" s="17" t="s">
@@ -1998,7 +1998,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E6" s="23"/>
       <c r="F6" s="20"/>
@@ -2025,16 +2025,16 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="18" t="s">
         <v>52</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2043,16 +2043,16 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="F11" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2061,16 +2061,16 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="F12" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2079,16 +2079,16 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>